<commit_message>
Updated excel documents with new paramters
</commit_message>
<xml_diff>
--- a/Painting Scavenger Hunt/xml/system parameters.xlsx
+++ b/Painting Scavenger Hunt/xml/system parameters.xlsx
@@ -23,38 +23,53 @@
   <connection id="2" name="hunt and painting" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\hunt and painting.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="3" name="importer" type="4" refreshedVersion="0" background="1">
+  <connection id="3" name="hunt1" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\hunt.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="4" name="importer" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\importer.xml" htmlTables="1"/>
   </connection>
-  <connection id="4" name="importer1" type="4" refreshedVersion="0" background="1">
+  <connection id="5" name="importer1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\importer.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="5" name="importer2" type="4" refreshedVersion="0" background="1">
+  <connection id="6" name="importer2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\importer.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="6" name="importer3" type="4" refreshedVersion="0" background="1">
+  <connection id="7" name="importer3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\importer.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="7" name="menu" type="4" refreshedVersion="0" background="1">
+  <connection id="8" name="importer4" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\importer.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="9" name="importer5" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\importer.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="10" name="importer6" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\importer.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="11" name="menu" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\menu.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="8" name="menu1" type="4" refreshedVersion="0" background="1">
+  <connection id="12" name="menu1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\menu.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="9" name="start-up" type="4" refreshedVersion="0" background="1">
+  <connection id="13" name="menu2" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\menu.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="14" name="start-up" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\start-up.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="10" name="start-up params" type="4" refreshedVersion="0" background="1">
+  <connection id="15" name="start-up params" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\start-up params.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="11" name="start-up params1" type="4" refreshedVersion="0" background="1">
+  <connection id="16" name="start-up params1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\start-up params.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
   <si>
     <t>hunt</t>
   </si>
@@ -71,9 +86,6 @@
     <t>Specification Files</t>
   </si>
   <si>
-    <t>interface</t>
-  </si>
-  <si>
     <t>game_info</t>
   </si>
   <si>
@@ -89,9 +101,6 @@
     <t>assets/interface/</t>
   </si>
   <si>
-    <t>assets/game_info/</t>
-  </si>
-  <si>
     <t>assets/ooi images/</t>
   </si>
   <si>
@@ -101,18 +110,6 @@
     <t>assets/end goal images/</t>
   </si>
   <si>
-    <t>Hunt Paramters</t>
-  </si>
-  <si>
-    <t>magnify_scale</t>
-  </si>
-  <si>
-    <t>magnify_radius</t>
-  </si>
-  <si>
-    <t>hunt_count</t>
-  </si>
-  <si>
     <t>Menu Parameters</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>importer.xml</t>
   </si>
   <si>
-    <t>hunt.xml</t>
-  </si>
-  <si>
     <t>menu.xml</t>
   </si>
   <si>
@@ -156,6 +150,123 @@
   </si>
   <si>
     <t>xml/painting.xml</t>
+  </si>
+  <si>
+    <t>canvas_rectangle</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>game_interface</t>
+  </si>
+  <si>
+    <t>menu_border</t>
+  </si>
+  <si>
+    <t>menu_opacity</t>
+  </si>
+  <si>
+    <t>text_format</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>bold</t>
+  </si>
+  <si>
+    <t>italic</t>
+  </si>
+  <si>
+    <t>text_button_color</t>
+  </si>
+  <si>
+    <t>up_color</t>
+  </si>
+  <si>
+    <t>over_color</t>
+  </si>
+  <si>
+    <t>down_color</t>
+  </si>
+  <si>
+    <t>0x836A35</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>caption</t>
+  </si>
+  <si>
+    <t>text_button</t>
+  </si>
+  <si>
+    <t>link_usable</t>
+  </si>
+  <si>
+    <t>link_unusable</t>
+  </si>
+  <si>
+    <t>link_accentuated</t>
+  </si>
+  <si>
+    <t>0xEEBB55</t>
+  </si>
+  <si>
+    <t>0xCC9933</t>
+  </si>
+  <si>
+    <t>0xFE5E5A</t>
+  </si>
+  <si>
+    <t>0xE5E5E5</t>
+  </si>
+  <si>
+    <t>assets/game info/</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Initial Values</t>
+  </si>
+  <si>
+    <t>loading screen</t>
+  </si>
+  <si>
+    <t>loading_title</t>
+  </si>
+  <si>
+    <t>The Night Before the Battle Interactive Scavenger Hunt</t>
+  </si>
+  <si>
+    <t>stage_size</t>
   </si>
 </sst>
 </file>
@@ -224,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -233,8 +344,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -248,33 +364,53 @@
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
   <Schema ID="Schema4">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="Hunt">
-        <xsd:complexType>
-          <xsd:attribute name="magnify_scale" form="unqualified" type="xsd:integer"/>
-          <xsd:attribute name="magnify_radius" form="unqualified" type="xsd:integer"/>
-          <xsd:attribute name="hunt_count" form="unqualified" type="xsd:integer"/>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
-  <Schema ID="Schema7">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="Menu">
         <xsd:complexType>
           <xsd:sequence minOccurs="0">
             <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="menu_color" form="unqualified"/>
+            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="menu_border" form="unqualified"/>
+            <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="menu_opacity" form="unqualified"/>
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="text_format" form="unqualified">
+              <xsd:complexType>
+                <xsd:all>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="size" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="color" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="bold" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="italic" form="unqualified"/>
+                </xsd:all>
+                <xsd:attribute name="name" form="unqualified" type="xsd:string"/>
+              </xsd:complexType>
+            </xsd:element>
+            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="up_color" form="unqualified"/>
+            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="over_color" form="unqualified"/>
+            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="down_color" form="unqualified"/>
           </xsd:sequence>
         </xsd:complexType>
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Schema ID="Schema8">
+  <Schema ID="Schema5">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="Importer">
         <xsd:complexType>
           <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="loading_title" form="unqualified"/>
+            <xsd:element minOccurs="0" nillable="true" name="stage_size" form="unqualified">
+              <xsd:complexType>
+                <xsd:attribute name="width" form="unqualified" type="xsd:integer"/>
+                <xsd:attribute name="height" form="unqualified" type="xsd:integer"/>
+              </xsd:complexType>
+            </xsd:element>
+            <xsd:element minOccurs="0" nillable="true" name="canvas_rectangle" form="unqualified">
+              <xsd:complexType>
+                <xsd:attribute name="x" form="unqualified" type="xsd:integer"/>
+                <xsd:attribute name="y" form="unqualified" type="xsd:integer"/>
+                <xsd:attribute name="width" form="unqualified" type="xsd:integer"/>
+                <xsd:attribute name="height" form="unqualified" type="xsd:integer"/>
+              </xsd:complexType>
+            </xsd:element>
+            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="menu" form="unqualified"/>
             <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="about" form="unqualified"/>
-            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="menu" form="unqualified"/>
             <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="hunt" form="unqualified"/>
             <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="painting" form="unqualified"/>
             <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="objects_of_interest" form="unqualified"/>
@@ -282,7 +418,7 @@
             <xsd:element minOccurs="0" nillable="true" name="Asset_Directories" form="unqualified">
               <xsd:complexType>
                 <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="interface" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="game_interface" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="game_info" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="object_of_interest_images" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="object_of_interest_info" form="unqualified"/>
@@ -295,93 +431,164 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="8" Name="Hunt_Map" RootElement="Hunt" SchemaID="Schema4" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
+  <Map ID="18" Name="Importer_Map" RootElement="Importer" SchemaID="Schema5" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="10" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="11" Name="Importer_Map" RootElement="Importer" SchemaID="Schema8" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="6" DataBindingLoadMode="1"/>
-  </Map>
-  <Map ID="10" Name="Menu_Map" RootElement="Menu" SchemaID="Schema7" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="8" DataBindingLoadMode="1"/>
+  <Map ID="13" Name="Menu_Map" RootElement="Menu" SchemaID="Schema4" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="13" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table26" displayName="Table26" ref="A42:E49" tableType="xml" totalsRowShown="0" connectionId="13">
+  <autoFilter ref="A42:E49">
+    <filterColumn colId="1"/>
+    <filterColumn colId="2"/>
+    <filterColumn colId="3"/>
+    <filterColumn colId="4"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" uniqueName="name" name="name">
+      <xmlColumnPr mapId="13" xpath="/Menu/text_format/@name" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" uniqueName="size" name="size">
+      <xmlColumnPr mapId="13" xpath="/Menu/text_format/size" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="3" uniqueName="color" name="color">
+      <xmlColumnPr mapId="13" xpath="/Menu/text_format/color" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="4" uniqueName="bold" name="bold">
+      <xmlColumnPr mapId="13" xpath="/Menu/text_format/bold" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="5" uniqueName="italic" name="italic">
+      <xmlColumnPr mapId="13" xpath="/Menu/text_format/italic" xmlDataType="string"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/tableSingleCells1.xml><?xml version="1.0" encoding="utf-8"?>
 <singleXmlCells xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <singleXmlCell id="1" r="B21" connectionId="1">
-    <xmlCellPr id="1" uniqueName="magnify_scale">
-      <xmlPr mapId="8" xpath="/Hunt/@magnify_scale" xmlDataType="integer"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="2" r="B22" connectionId="1">
-    <xmlCellPr id="1" uniqueName="magnify_radius">
-      <xmlPr mapId="8" xpath="/Hunt/@magnify_radius" xmlDataType="integer"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="3" r="B23" connectionId="1">
-    <xmlCellPr id="1" uniqueName="hunt_count">
-      <xmlPr mapId="8" xpath="/Hunt/@hunt_count" xmlDataType="integer"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="13" r="B28" connectionId="8">
+  <singleXmlCell id="23" r="B37" connectionId="13">
     <xmlCellPr id="1" uniqueName="menu_color">
-      <xmlPr mapId="10" xpath="/Menu/menu_color" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="14" r="B3" connectionId="6">
+      <xmlPr mapId="13" xpath="/Menu/menu_color" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="24" r="B38" connectionId="13">
+    <xmlCellPr id="1" uniqueName="menu_border">
+      <xmlPr mapId="13" xpath="/Menu/menu_border" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="25" r="B39" connectionId="13">
+    <xmlCellPr id="1" uniqueName="menu_opacity">
+      <xmlPr mapId="13" xpath="/Menu/menu_opacity" xmlDataType="double"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="28" r="B52" connectionId="13">
+    <xmlCellPr id="1" uniqueName="up_color">
+      <xmlPr mapId="13" xpath="/Menu/up_color" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="29" r="B53" connectionId="13">
+    <xmlCellPr id="1" uniqueName="over_color">
+      <xmlPr mapId="13" xpath="/Menu/over_color" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="30" r="B54" connectionId="13">
+    <xmlCellPr id="1" uniqueName="down_color">
+      <xmlPr mapId="13" xpath="/Menu/down_color" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="19" r="B3" connectionId="10">
+    <xmlCellPr id="1" uniqueName="loading_title">
+      <xmlPr mapId="18" xpath="/Importer/loading_title" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="20" r="B10" connectionId="10">
+    <xmlCellPr id="1" uniqueName="x">
+      <xmlPr mapId="18" xpath="/Importer/canvas_rectangle/@x" xmlDataType="integer"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="21" r="B6" connectionId="10">
+    <xmlCellPr id="1" uniqueName="width">
+      <xmlPr mapId="18" xpath="/Importer/stage_size/@width" xmlDataType="integer"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="22" r="B7" connectionId="10">
+    <xmlCellPr id="1" uniqueName="height">
+      <xmlPr mapId="18" xpath="/Importer/stage_size/@height" xmlDataType="integer"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="27" r="B11" connectionId="10">
+    <xmlCellPr id="1" uniqueName="y">
+      <xmlPr mapId="18" xpath="/Importer/canvas_rectangle/@y" xmlDataType="integer"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="31" r="B12" connectionId="10">
+    <xmlCellPr id="1" uniqueName="width">
+      <xmlPr mapId="18" xpath="/Importer/canvas_rectangle/@width" xmlDataType="integer"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="32" r="B13" connectionId="10">
+    <xmlCellPr id="1" uniqueName="height">
+      <xmlPr mapId="18" xpath="/Importer/canvas_rectangle/@height" xmlDataType="integer"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="33" r="B18" connectionId="10">
+    <xmlCellPr id="1" uniqueName="menu">
+      <xmlPr mapId="18" xpath="/Importer/menu" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="34" r="B19" connectionId="10">
     <xmlCellPr id="1" uniqueName="about">
-      <xmlPr mapId="11" xpath="/Importer/about" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="15" r="B2" connectionId="6">
-    <xmlCellPr id="1" uniqueName="menu">
-      <xmlPr mapId="11" xpath="/Importer/menu" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="16" r="B4" connectionId="6">
+      <xmlPr mapId="18" xpath="/Importer/about" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="35" r="B20" connectionId="10">
     <xmlCellPr id="1" uniqueName="hunt">
-      <xmlPr mapId="11" xpath="/Importer/hunt" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="17" r="B5" connectionId="6">
+      <xmlPr mapId="18" xpath="/Importer/hunt" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="36" r="B21" connectionId="10">
     <xmlCellPr id="1" uniqueName="painting">
-      <xmlPr mapId="11" xpath="/Importer/painting" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="18" r="B6" connectionId="6">
+      <xmlPr mapId="18" xpath="/Importer/painting" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="37" r="B22" connectionId="10">
     <xmlCellPr id="1" uniqueName="objects_of_interest">
-      <xmlPr mapId="11" xpath="/Importer/objects_of_interest" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="19" r="B7" connectionId="6">
+      <xmlPr mapId="18" xpath="/Importer/objects_of_interest" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="38" r="B23" connectionId="10">
     <xmlCellPr id="1" uniqueName="end_goal">
-      <xmlPr mapId="11" xpath="/Importer/end_goal" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="20" r="B12" connectionId="6">
-    <xmlCellPr id="1" uniqueName="interface">
-      <xmlPr mapId="11" xpath="/Importer/Asset_Directories/interface" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="21" r="B13" connectionId="6">
+      <xmlPr mapId="18" xpath="/Importer/end_goal" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="39" r="B28" connectionId="10">
+    <xmlCellPr id="1" uniqueName="game_interface">
+      <xmlPr mapId="18" xpath="/Importer/Asset_Directories/game_interface" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="40" r="B29" connectionId="10">
     <xmlCellPr id="1" uniqueName="game_info">
-      <xmlPr mapId="11" xpath="/Importer/Asset_Directories/game_info" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="22" r="B14" connectionId="6">
+      <xmlPr mapId="18" xpath="/Importer/Asset_Directories/game_info" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="41" r="B30" connectionId="10">
     <xmlCellPr id="1" uniqueName="object_of_interest_images">
-      <xmlPr mapId="11" xpath="/Importer/Asset_Directories/object_of_interest_images" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="23" r="B15" connectionId="6">
+      <xmlPr mapId="18" xpath="/Importer/Asset_Directories/object_of_interest_images" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="42" r="B31" connectionId="10">
     <xmlCellPr id="1" uniqueName="object_of_interest_info">
-      <xmlPr mapId="11" xpath="/Importer/Asset_Directories/object_of_interest_info" xmlDataType="string"/>
-    </xmlCellPr>
-  </singleXmlCell>
-  <singleXmlCell id="24" r="B16" connectionId="6">
+      <xmlPr mapId="18" xpath="/Importer/Asset_Directories/object_of_interest_info" xmlDataType="string"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="43" r="B32" connectionId="10">
     <xmlCellPr id="1" uniqueName="end_goal_images">
-      <xmlPr mapId="11" xpath="/Importer/Asset_Directories/end_goal_images" xmlDataType="string"/>
+      <xmlPr mapId="18" xpath="/Importer/Asset_Directories/end_goal_images" xmlDataType="string"/>
     </xmlCellPr>
   </singleXmlCell>
 </singleXmlCells>
@@ -672,174 +879,413 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>31</v>
+      <c r="A2" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
+      <c r="A5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1265</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="18.75">
-      <c r="A11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="B7" s="4">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="9">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="B12" s="9">
+        <v>765</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="18.75">
-      <c r="A20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="9">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="18.75">
+      <c r="A17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="4">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="4">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="18.75">
+      <c r="A27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B23" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="18.75">
-      <c r="A27" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="18.75">
+      <c r="A36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" t="s">
+        <v>39</v>
+      </c>
+      <c r="E42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="8">
+        <v>30</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44">
+        <v>24</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45">
         <v>20</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>21</v>
+      <c r="C45" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46">
+        <v>30</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47">
+        <v>20</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48">
+        <v>20</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="8">
+        <v>20</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>